<commit_message>
Projeto finalizado, até então sem erros encontrados.
</commit_message>
<xml_diff>
--- a/projetos-python/projeto-4-bi/NOTASFINAISALUNOS.xlsx
+++ b/projetos-python/projeto-4-bi/NOTASFINAISALUNOS.xlsx
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>111111</t>
+          <t>123456</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -500,28 +500,28 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>654321</t>
+          <t>000111</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Daniela</t>
+          <t>thiago</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
         <v>3</v>
       </c>
-      <c r="E3" t="n">
-        <v>2</v>
-      </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G3" t="n">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização, pois não estava seguindo as corretas orientações do projeto.
</commit_message>
<xml_diff>
--- a/projetos-python/projeto-4-bi/NOTASFINAISALUNOS.xlsx
+++ b/projetos-python/projeto-4-bi/NOTASFINAISALUNOS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,55 +473,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>123456</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>thiago</t>
+          <t>Thiago</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G2" t="n">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>000111</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>thiago</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" t="n">
-        <v>4</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2.5</v>
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projeto a principio finalizado
</commit_message>
<xml_diff>
--- a/projetos-python/projeto-4-bi/NOTASFINAISALUNOS.xlsx
+++ b/projetos-python/projeto-4-bi/NOTASFINAISALUNOS.xlsx
@@ -473,28 +473,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Thiago</t>
+          <t>Lara</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G2" t="n">
-        <v>7.5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>